<commit_message>
sample set geojson created
</commit_message>
<xml_diff>
--- a/docs/business_by_year_range_A_Gl.xlsx
+++ b/docs/business_by_year_range_A_Gl.xlsx
@@ -1312,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>